<commit_message>
new skill types, and more edge definitions
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="284">
   <si>
     <t>ALERTNESS</t>
   </si>
@@ -853,6 +853,27 @@
   </si>
   <si>
     <t>skill</t>
+  </si>
+  <si>
+    <t>Battle</t>
+  </si>
+  <si>
+    <t>Arcana</t>
+  </si>
+  <si>
+    <t>FAITH</t>
+  </si>
+  <si>
+    <t>PSIONICS</t>
+  </si>
+  <si>
+    <t>SPELLCASTING</t>
+  </si>
+  <si>
+    <t>WEIRD_SCIENCE</t>
+  </si>
+  <si>
+    <t>ANY</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1184,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4875,10 +4896,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C141"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4888,7 +4909,7 @@
     <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>237</v>
       </c>
@@ -4899,769 +4920,657 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>268</v>
+      </c>
+      <c r="C11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>261</v>
+      </c>
+      <c r="C13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>279</v>
+      </c>
+      <c r="C19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" t="s">
+        <v>250</v>
+      </c>
+      <c r="D22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C23" t="s">
+        <v>250</v>
+      </c>
+      <c r="D23" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
+        <v>279</v>
+      </c>
+      <c r="C24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>266</v>
+      </c>
+      <c r="C27" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>263</v>
+      </c>
+      <c r="C28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>280</v>
+      </c>
+      <c r="C29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>266</v>
+      </c>
+      <c r="C30" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>282</v>
+      </c>
+      <c r="C31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C32" t="s">
+        <v>250</v>
+      </c>
+      <c r="D32" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" t="s">
+        <v>250</v>
+      </c>
+      <c r="D33" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
+        <v>254</v>
+      </c>
+      <c r="C34" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>262</v>
+      </c>
+      <c r="C35" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>269</v>
+      </c>
+      <c r="C36" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>261</v>
+      </c>
+      <c r="C37" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>281</v>
+      </c>
+      <c r="C38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>271</v>
+      </c>
+      <c r="C39" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>275</v>
+      </c>
+      <c r="C40" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
+        <v>259</v>
+      </c>
+      <c r="C41" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
+        <v>273</v>
+      </c>
+      <c r="C42" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" t="s">
         <v>256</v>
       </c>
-      <c r="C24" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C43" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
         <v>256</v>
       </c>
-      <c r="C29" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>253</v>
+      </c>
+      <c r="B50" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>254</v>
+      </c>
+      <c r="B51" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>255</v>
+      </c>
+      <c r="B52" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>279</v>
+      </c>
+      <c r="B53" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>256</v>
       </c>
-      <c r="C38" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" t="s">
-        <v>256</v>
-      </c>
-      <c r="C39" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" t="s">
-        <v>256</v>
-      </c>
-      <c r="C49" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" t="s">
-        <v>256</v>
-      </c>
-      <c r="C50" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>49</v>
-      </c>
       <c r="B54" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>268</v>
       </c>
-      <c r="C54" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" t="s">
-        <v>256</v>
-      </c>
-      <c r="C56" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" t="s">
-        <v>256</v>
-      </c>
-      <c r="C58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" t="s">
-        <v>268</v>
-      </c>
-      <c r="C59" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" t="s">
-        <v>261</v>
-      </c>
-      <c r="C69" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>253</v>
-      </c>
-      <c r="B119" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>254</v>
-      </c>
-      <c r="B120" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>255</v>
-      </c>
-      <c r="B121" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>256</v>
-      </c>
-      <c r="B122" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>257</v>
-      </c>
-      <c r="B123" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B113">
-      <formula1>$A$119:$A$141</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B44">
+      <formula1>$A$50:$A$76</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C113">
-      <formula1>$B$119:$B$123</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C44">
+      <formula1>$B$50:$B$54</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
definition of edges from rifts book, including prereqs, but without descriptions
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="defs" sheetId="1" r:id="rId1"/>
-    <sheet name="edge_prereq" sheetId="2" r:id="rId2"/>
-    <sheet name="attr_prereq" sheetId="3" r:id="rId3"/>
-    <sheet name="skill_prereq" sheetId="4" r:id="rId4"/>
+    <sheet name="framework_prereq" sheetId="5" r:id="rId2"/>
+    <sheet name="edge_prereq" sheetId="2" r:id="rId3"/>
+    <sheet name="attr_prereq" sheetId="3" r:id="rId4"/>
+    <sheet name="skill_prereq" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="347">
   <si>
     <t>ALERTNESS</t>
   </si>
@@ -773,9 +774,6 @@
     <t>VIGOR</t>
   </si>
   <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>D6</t>
   </si>
   <si>
@@ -785,24 +783,12 @@
     <t>D12</t>
   </si>
   <si>
-    <t>BOATING</t>
-  </si>
-  <si>
     <t>CLIMBING</t>
   </si>
   <si>
-    <t>DRIVING</t>
-  </si>
-  <si>
     <t>FIGHTING</t>
   </si>
   <si>
-    <t>GAMBLING</t>
-  </si>
-  <si>
-    <t>HEALING</t>
-  </si>
-  <si>
     <t>INTIMIDATION</t>
   </si>
   <si>
@@ -827,9 +813,6 @@
     <t>REPAIR</t>
   </si>
   <si>
-    <t>RIDING</t>
-  </si>
-  <si>
     <t>SHOOTING</t>
   </si>
   <si>
@@ -842,27 +825,15 @@
     <t>SURVIVAL</t>
   </si>
   <si>
-    <t>SWIMMING</t>
-  </si>
-  <si>
     <t>TAUNT</t>
   </si>
   <si>
-    <t>THROWING</t>
-  </si>
-  <si>
     <t>TRACKING</t>
   </si>
   <si>
     <t>skill</t>
   </si>
   <si>
-    <t>Battle</t>
-  </si>
-  <si>
-    <t>Arcana</t>
-  </si>
-  <si>
     <t>FAITH</t>
   </si>
   <si>
@@ -1053,6 +1024,51 @@
   </si>
   <si>
     <t>ICONIC</t>
+  </si>
+  <si>
+    <t>SQL (needs to include the knowledge_type(sp?) column that's in the knowledge-skills branch)</t>
+  </si>
+  <si>
+    <t>framework</t>
+  </si>
+  <si>
+    <t>COMBAT_CYBORG</t>
+  </si>
+  <si>
+    <t>MARS</t>
+  </si>
+  <si>
+    <t>JUICER</t>
+  </si>
+  <si>
+    <t>CYBER_KNIGHT</t>
+  </si>
+  <si>
+    <t>BURSTER</t>
+  </si>
+  <si>
+    <t>CRAZY</t>
+  </si>
+  <si>
+    <t>LEY_LINE_WALKER</t>
+  </si>
+  <si>
+    <t>HOW TO HANDLE GENERIC ARCANEBACKGROUND???</t>
+  </si>
+  <si>
+    <t>also has a power prereq: telekinesis</t>
+  </si>
+  <si>
+    <t>also has a power prereq: smite</t>
+  </si>
+  <si>
+    <t>also has a power prereq: telepathy</t>
+  </si>
+  <si>
+    <t>ARCANA</t>
+  </si>
+  <si>
+    <t>BATTLE</t>
   </si>
 </sst>
 </file>
@@ -1383,10 +1399,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H167"/>
+  <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,7 +1441,7 @@
         <v>232</v>
       </c>
       <c r="H1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1805,7 +1822,7 @@
         <v>132</v>
       </c>
       <c r="E15" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="F15" t="s">
         <v>230</v>
@@ -3485,7 +3502,7 @@
         <v>190</v>
       </c>
       <c r="E75" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="F75" t="s">
         <v>230</v>
@@ -3516,10 +3533,10 @@
         <v>230</v>
       </c>
       <c r="F76" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G76" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="H76" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3544,7 +3561,7 @@
         <v>230</v>
       </c>
       <c r="F77" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G77" t="s">
         <v>230</v>
@@ -3569,10 +3586,10 @@
         <v>193</v>
       </c>
       <c r="E78" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="F78" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G78" t="s">
         <v>230</v>
@@ -3600,7 +3617,7 @@
         <v>230</v>
       </c>
       <c r="F79" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G79" t="s">
         <v>230</v>
@@ -3656,7 +3673,7 @@
         <v>230</v>
       </c>
       <c r="F81" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G81" t="s">
         <v>230</v>
@@ -3712,7 +3729,7 @@
         <v>230</v>
       </c>
       <c r="F83" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G83" t="s">
         <v>230</v>
@@ -3768,7 +3785,7 @@
         <v>230</v>
       </c>
       <c r="F85" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G85" t="s">
         <v>230</v>
@@ -3824,7 +3841,7 @@
         <v>230</v>
       </c>
       <c r="F87" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G87" t="s">
         <v>230</v>
@@ -3852,7 +3869,7 @@
         <v>230</v>
       </c>
       <c r="F88" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G88" t="s">
         <v>230</v>
@@ -3880,7 +3897,7 @@
         <v>230</v>
       </c>
       <c r="F89" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G89" t="s">
         <v>230</v>
@@ -3992,7 +4009,7 @@
         <v>230</v>
       </c>
       <c r="F93" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G93" t="s">
         <v>230</v>
@@ -4535,377 +4552,1102 @@
 SET @MASTER_OF_ARMS_ID = LAST_INSERT_ID();</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>277</v>
+      </c>
+      <c r="B114" t="s">
+        <v>331</v>
+      </c>
+      <c r="C114" t="s">
+        <v>120</v>
+      </c>
+      <c r="E114" t="s">
+        <v>230</v>
+      </c>
+      <c r="F114" t="s">
+        <v>230</v>
+      </c>
+      <c r="G114" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>278</v>
+      </c>
+      <c r="B115" t="s">
+        <v>331</v>
+      </c>
+      <c r="C115" t="s">
+        <v>228</v>
+      </c>
+      <c r="E115" t="s">
+        <v>230</v>
+      </c>
+      <c r="F115" t="s">
+        <v>230</v>
+      </c>
+      <c r="G115" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>279</v>
+      </c>
+      <c r="B116" t="s">
+        <v>331</v>
+      </c>
+      <c r="C116" t="s">
+        <v>116</v>
+      </c>
+      <c r="E116" t="s">
+        <v>230</v>
+      </c>
+      <c r="F116" t="s">
+        <v>230</v>
+      </c>
+      <c r="G116" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>280</v>
+      </c>
+      <c r="B117" t="s">
+        <v>331</v>
+      </c>
+      <c r="C117" t="s">
+        <v>119</v>
+      </c>
+      <c r="E117" t="s">
+        <v>230</v>
+      </c>
+      <c r="F117" t="s">
+        <v>230</v>
+      </c>
+      <c r="G117" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>281</v>
+      </c>
+      <c r="B118" t="s">
+        <v>331</v>
+      </c>
+      <c r="C118" t="s">
+        <v>120</v>
+      </c>
+      <c r="E118" t="s">
+        <v>230</v>
+      </c>
+      <c r="F118" t="s">
+        <v>230</v>
+      </c>
+      <c r="G118" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>282</v>
+      </c>
+      <c r="B119" t="s">
+        <v>331</v>
+      </c>
+      <c r="C119" t="s">
+        <v>119</v>
+      </c>
+      <c r="E119" t="s">
+        <v>230</v>
+      </c>
+      <c r="F119" t="s">
+        <v>230</v>
+      </c>
+      <c r="G119" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>283</v>
+      </c>
+      <c r="B120" t="s">
+        <v>331</v>
+      </c>
+      <c r="C120" t="s">
+        <v>121</v>
+      </c>
+      <c r="E120" t="s">
+        <v>230</v>
+      </c>
+      <c r="F120" t="s">
+        <v>230</v>
+      </c>
+      <c r="G120" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>284</v>
+      </c>
+      <c r="B121" t="s">
+        <v>331</v>
+      </c>
+      <c r="C121" t="s">
+        <v>116</v>
+      </c>
+      <c r="E121" t="s">
+        <v>230</v>
+      </c>
+      <c r="F121" t="s">
+        <v>230</v>
+      </c>
+      <c r="G121" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>285</v>
+      </c>
+      <c r="B122" t="s">
+        <v>331</v>
+      </c>
+      <c r="C122" t="s">
+        <v>119</v>
+      </c>
+      <c r="E122" t="s">
+        <v>230</v>
+      </c>
+      <c r="F122" t="s">
+        <v>230</v>
+      </c>
+      <c r="G122" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>286</v>
+      </c>
+      <c r="B123" t="s">
+        <v>331</v>
+      </c>
+      <c r="C123" t="s">
+        <v>228</v>
+      </c>
+      <c r="E123" t="s">
+        <v>230</v>
+      </c>
+      <c r="F123" t="s">
+        <v>230</v>
+      </c>
+      <c r="G123" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>287</v>
       </c>
-      <c r="B114" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="B124" t="s">
+        <v>331</v>
+      </c>
+      <c r="C124" t="s">
+        <v>228</v>
+      </c>
+      <c r="E124" t="s">
+        <v>230</v>
+      </c>
+      <c r="F124" t="s">
+        <v>230</v>
+      </c>
+      <c r="G124" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>288</v>
       </c>
-      <c r="B115" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="B125" t="s">
+        <v>331</v>
+      </c>
+      <c r="C125" t="s">
+        <v>120</v>
+      </c>
+      <c r="E125" t="s">
+        <v>273</v>
+      </c>
+      <c r="F125" t="s">
+        <v>230</v>
+      </c>
+      <c r="G125" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>289</v>
       </c>
-      <c r="B116" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="B126" t="s">
+        <v>331</v>
+      </c>
+      <c r="C126" t="s">
+        <v>119</v>
+      </c>
+      <c r="E126" t="s">
+        <v>230</v>
+      </c>
+      <c r="F126" t="s">
+        <v>230</v>
+      </c>
+      <c r="G126" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>290</v>
       </c>
-      <c r="B117" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="B127" t="s">
+        <v>331</v>
+      </c>
+      <c r="C127" t="s">
+        <v>121</v>
+      </c>
+      <c r="E127" t="s">
+        <v>230</v>
+      </c>
+      <c r="F127" t="s">
+        <v>230</v>
+      </c>
+      <c r="G127" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>291</v>
       </c>
-      <c r="B118" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="B128" t="s">
+        <v>331</v>
+      </c>
+      <c r="C128" t="s">
+        <v>119</v>
+      </c>
+      <c r="E128" t="s">
+        <v>230</v>
+      </c>
+      <c r="F128" t="s">
+        <v>230</v>
+      </c>
+      <c r="G128" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>292</v>
       </c>
-      <c r="B119" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="B129" t="s">
+        <v>331</v>
+      </c>
+      <c r="C129" t="s">
+        <v>119</v>
+      </c>
+      <c r="E129" t="s">
+        <v>230</v>
+      </c>
+      <c r="F129" t="s">
+        <v>230</v>
+      </c>
+      <c r="G129" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>293</v>
       </c>
-      <c r="B120" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="B130" t="s">
+        <v>331</v>
+      </c>
+      <c r="C130" t="s">
+        <v>228</v>
+      </c>
+      <c r="E130" t="s">
+        <v>230</v>
+      </c>
+      <c r="F130" t="s">
+        <v>230</v>
+      </c>
+      <c r="G130" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>294</v>
       </c>
-      <c r="B121" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="B131" t="s">
+        <v>331</v>
+      </c>
+      <c r="C131" t="s">
+        <v>120</v>
+      </c>
+      <c r="E131" t="s">
+        <v>230</v>
+      </c>
+      <c r="F131" t="s">
+        <v>230</v>
+      </c>
+      <c r="G131" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>295</v>
       </c>
-      <c r="B122" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="B132" t="s">
+        <v>331</v>
+      </c>
+      <c r="C132" t="s">
+        <v>120</v>
+      </c>
+      <c r="E132" t="s">
+        <v>230</v>
+      </c>
+      <c r="F132" t="s">
+        <v>230</v>
+      </c>
+      <c r="G132" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>296</v>
       </c>
-      <c r="B123" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="B133" t="s">
+        <v>331</v>
+      </c>
+      <c r="C133" t="s">
+        <v>121</v>
+      </c>
+      <c r="E133" t="s">
+        <v>230</v>
+      </c>
+      <c r="F133" t="s">
+        <v>230</v>
+      </c>
+      <c r="G133" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>297</v>
       </c>
-      <c r="B124" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="B134" t="s">
+        <v>331</v>
+      </c>
+      <c r="C134" t="s">
+        <v>119</v>
+      </c>
+      <c r="E134" t="s">
+        <v>230</v>
+      </c>
+      <c r="F134" t="s">
+        <v>230</v>
+      </c>
+      <c r="G134" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>298</v>
       </c>
-      <c r="B125" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="B135" t="s">
+        <v>331</v>
+      </c>
+      <c r="C135" t="s">
+        <v>120</v>
+      </c>
+      <c r="E135" t="s">
+        <v>230</v>
+      </c>
+      <c r="F135" t="s">
+        <v>230</v>
+      </c>
+      <c r="G135" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>299</v>
       </c>
-      <c r="B126" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="B136" t="s">
+        <v>331</v>
+      </c>
+      <c r="C136" t="s">
+        <v>121</v>
+      </c>
+      <c r="E136" t="s">
+        <v>230</v>
+      </c>
+      <c r="F136" t="s">
+        <v>230</v>
+      </c>
+      <c r="G136" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>300</v>
       </c>
-      <c r="B127" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="B137" t="s">
+        <v>331</v>
+      </c>
+      <c r="C137" t="s">
+        <v>228</v>
+      </c>
+      <c r="E137" t="s">
+        <v>230</v>
+      </c>
+      <c r="F137" t="s">
+        <v>230</v>
+      </c>
+      <c r="G137" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>301</v>
       </c>
-      <c r="B128" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="B138" t="s">
+        <v>331</v>
+      </c>
+      <c r="C138" t="s">
+        <v>119</v>
+      </c>
+      <c r="E138" t="s">
+        <v>230</v>
+      </c>
+      <c r="F138" t="s">
+        <v>230</v>
+      </c>
+      <c r="G138" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>302</v>
       </c>
-      <c r="B129" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="B139" t="s">
+        <v>331</v>
+      </c>
+      <c r="C139" t="s">
+        <v>120</v>
+      </c>
+      <c r="E139" t="s">
+        <v>230</v>
+      </c>
+      <c r="F139" t="s">
+        <v>230</v>
+      </c>
+      <c r="G139" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>303</v>
       </c>
-      <c r="B130" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="B140" t="s">
+        <v>331</v>
+      </c>
+      <c r="C140" t="s">
+        <v>228</v>
+      </c>
+      <c r="E140" t="s">
+        <v>230</v>
+      </c>
+      <c r="F140" t="s">
+        <v>230</v>
+      </c>
+      <c r="G140" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>304</v>
       </c>
-      <c r="B131" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="B141" t="s">
+        <v>331</v>
+      </c>
+      <c r="C141" t="s">
+        <v>119</v>
+      </c>
+      <c r="E141" t="s">
+        <v>230</v>
+      </c>
+      <c r="F141" t="s">
+        <v>230</v>
+      </c>
+      <c r="G141" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>305</v>
       </c>
-      <c r="B132" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="B142" t="s">
+        <v>331</v>
+      </c>
+      <c r="C142" t="s">
+        <v>121</v>
+      </c>
+      <c r="E142" t="s">
+        <v>230</v>
+      </c>
+      <c r="F142" t="s">
+        <v>230</v>
+      </c>
+      <c r="G142" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>306</v>
       </c>
-      <c r="B133" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="B143" t="s">
+        <v>331</v>
+      </c>
+      <c r="C143" t="s">
+        <v>121</v>
+      </c>
+      <c r="E143" t="s">
+        <v>230</v>
+      </c>
+      <c r="F143" t="s">
+        <v>230</v>
+      </c>
+      <c r="G143" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>307</v>
       </c>
-      <c r="B134" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="B144" t="s">
+        <v>331</v>
+      </c>
+      <c r="C144" t="s">
+        <v>119</v>
+      </c>
+      <c r="E144" t="s">
+        <v>230</v>
+      </c>
+      <c r="F144" t="s">
+        <v>230</v>
+      </c>
+      <c r="G144" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>308</v>
-      </c>
-      <c r="B135" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>309</v>
-      </c>
-      <c r="B136" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>310</v>
-      </c>
-      <c r="B137" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>311</v>
-      </c>
-      <c r="B138" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>312</v>
-      </c>
-      <c r="B139" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>313</v>
-      </c>
-      <c r="B140" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>314</v>
-      </c>
-      <c r="B141" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>315</v>
-      </c>
-      <c r="B142" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>316</v>
-      </c>
-      <c r="B143" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>317</v>
-      </c>
-      <c r="B144" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>318</v>
       </c>
       <c r="B145" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>228</v>
+      </c>
+      <c r="E145" t="s">
+        <v>230</v>
+      </c>
+      <c r="F145" t="s">
+        <v>230</v>
+      </c>
+      <c r="G145" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>309</v>
+      </c>
+      <c r="B146" t="s">
+        <v>110</v>
+      </c>
+      <c r="C146" t="s">
+        <v>119</v>
+      </c>
+      <c r="E146" t="s">
+        <v>273</v>
+      </c>
+      <c r="F146" t="s">
+        <v>230</v>
+      </c>
+      <c r="G146" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>310</v>
+      </c>
+      <c r="B147" t="s">
+        <v>110</v>
+      </c>
+      <c r="C147" t="s">
+        <v>119</v>
+      </c>
+      <c r="E147" t="s">
+        <v>230</v>
+      </c>
+      <c r="F147" t="s">
+        <v>230</v>
+      </c>
+      <c r="G147" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>311</v>
+      </c>
+      <c r="B148" t="s">
+        <v>110</v>
+      </c>
+      <c r="C148" t="s">
+        <v>120</v>
+      </c>
+      <c r="E148" t="s">
+        <v>230</v>
+      </c>
+      <c r="F148" t="s">
+        <v>230</v>
+      </c>
+      <c r="G148" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>312</v>
+      </c>
+      <c r="B149" t="s">
+        <v>110</v>
+      </c>
+      <c r="C149" t="s">
+        <v>119</v>
+      </c>
+      <c r="E149" t="s">
+        <v>230</v>
+      </c>
+      <c r="F149" t="s">
+        <v>273</v>
+      </c>
+      <c r="G149" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>313</v>
+      </c>
+      <c r="B150" t="s">
+        <v>110</v>
+      </c>
+      <c r="C150" t="s">
+        <v>120</v>
+      </c>
+      <c r="E150" t="s">
+        <v>230</v>
+      </c>
+      <c r="F150" t="s">
+        <v>230</v>
+      </c>
+      <c r="G150" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>314</v>
+      </c>
+      <c r="B151" t="s">
+        <v>110</v>
+      </c>
+      <c r="C151" t="s">
+        <v>119</v>
+      </c>
+      <c r="E151" t="s">
+        <v>230</v>
+      </c>
+      <c r="F151" t="s">
+        <v>230</v>
+      </c>
+      <c r="G151" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>315</v>
+      </c>
+      <c r="B152" t="s">
+        <v>110</v>
+      </c>
+      <c r="C152" t="s">
+        <v>119</v>
+      </c>
+      <c r="E152" t="s">
+        <v>230</v>
+      </c>
+      <c r="F152" t="s">
+        <v>230</v>
+      </c>
+      <c r="G152" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>316</v>
+      </c>
+      <c r="B153" t="s">
+        <v>112</v>
+      </c>
+      <c r="C153" t="s">
+        <v>119</v>
+      </c>
+      <c r="E153" t="s">
+        <v>273</v>
+      </c>
+      <c r="F153" t="s">
+        <v>230</v>
+      </c>
+      <c r="G153" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>317</v>
+      </c>
+      <c r="B154" t="s">
+        <v>112</v>
+      </c>
+      <c r="C154" t="s">
+        <v>120</v>
+      </c>
+      <c r="E154" t="s">
+        <v>230</v>
+      </c>
+      <c r="F154" t="s">
+        <v>230</v>
+      </c>
+      <c r="G154" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>318</v>
+      </c>
+      <c r="B155" t="s">
+        <v>112</v>
+      </c>
+      <c r="C155" t="s">
+        <v>119</v>
+      </c>
+      <c r="E155" t="s">
+        <v>230</v>
+      </c>
+      <c r="F155" t="s">
+        <v>230</v>
+      </c>
+      <c r="G155" t="s">
+        <v>230</v>
+      </c>
+      <c r="H155" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B156" t="s">
+        <v>112</v>
+      </c>
+      <c r="C156" t="s">
+        <v>119</v>
+      </c>
+      <c r="E156" t="s">
+        <v>230</v>
+      </c>
+      <c r="F156" t="s">
+        <v>230</v>
+      </c>
+      <c r="G156" t="s">
+        <v>230</v>
+      </c>
+      <c r="H156" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="B157" t="s">
+        <v>112</v>
+      </c>
+      <c r="C157" t="s">
+        <v>120</v>
+      </c>
+      <c r="E157" t="s">
+        <v>230</v>
+      </c>
+      <c r="F157" t="s">
+        <v>230</v>
+      </c>
+      <c r="G157" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="B158" t="s">
+        <v>112</v>
+      </c>
+      <c r="C158" t="s">
+        <v>120</v>
+      </c>
+      <c r="E158" t="s">
+        <v>230</v>
+      </c>
+      <c r="F158" t="s">
+        <v>230</v>
+      </c>
+      <c r="G158" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>322</v>
       </c>
-      <c r="C149" t="s">
+      <c r="B159" t="s">
+        <v>112</v>
+      </c>
+      <c r="C159" t="s">
+        <v>119</v>
+      </c>
+      <c r="E159" t="s">
+        <v>230</v>
+      </c>
+      <c r="F159" t="s">
+        <v>230</v>
+      </c>
+      <c r="G159" t="s">
+        <v>230</v>
+      </c>
+      <c r="H159" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>323</v>
+      </c>
+      <c r="B160" t="s">
+        <v>99</v>
+      </c>
+      <c r="C160" t="s">
+        <v>119</v>
+      </c>
+      <c r="E160" t="s">
+        <v>230</v>
+      </c>
+      <c r="F160" t="s">
+        <v>230</v>
+      </c>
+      <c r="G160" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>324</v>
+      </c>
+      <c r="B161" t="s">
+        <v>99</v>
+      </c>
+      <c r="C161" t="s">
+        <v>119</v>
+      </c>
+      <c r="E161" t="s">
+        <v>273</v>
+      </c>
+      <c r="F161" t="s">
+        <v>230</v>
+      </c>
+      <c r="G161" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>325</v>
+      </c>
+      <c r="B162" t="s">
+        <v>99</v>
+      </c>
+      <c r="C162" t="s">
+        <v>119</v>
+      </c>
+      <c r="E162" t="s">
+        <v>230</v>
+      </c>
+      <c r="F162" t="s">
+        <v>230</v>
+      </c>
+      <c r="G162" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>326</v>
+      </c>
+      <c r="B163" t="s">
+        <v>99</v>
+      </c>
+      <c r="C163" t="s">
+        <v>119</v>
+      </c>
+      <c r="E163" t="s">
+        <v>230</v>
+      </c>
+      <c r="F163" t="s">
+        <v>273</v>
+      </c>
+      <c r="G163" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>327</v>
+      </c>
+      <c r="B164" t="s">
+        <v>99</v>
+      </c>
+      <c r="C164" t="s">
+        <v>228</v>
+      </c>
+      <c r="E164" t="s">
+        <v>273</v>
+      </c>
+      <c r="F164" t="s">
+        <v>230</v>
+      </c>
+      <c r="G164" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" t="s">
+        <v>99</v>
+      </c>
+      <c r="C165" t="s">
+        <v>228</v>
+      </c>
+      <c r="E165" t="s">
+        <v>273</v>
+      </c>
+      <c r="F165" t="s">
+        <v>230</v>
+      </c>
+      <c r="G165" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>329</v>
+      </c>
+      <c r="B166" t="s">
+        <v>113</v>
+      </c>
+      <c r="C166" t="s">
+        <v>228</v>
+      </c>
+      <c r="E166" t="s">
+        <v>230</v>
+      </c>
+      <c r="F166" t="s">
+        <v>273</v>
+      </c>
+      <c r="G166" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>330</v>
+      </c>
+      <c r="B167" t="s">
+        <v>113</v>
+      </c>
+      <c r="C167" t="s">
+        <v>228</v>
+      </c>
+      <c r="E167" t="s">
+        <v>230</v>
+      </c>
+      <c r="F167" t="s">
+        <v>230</v>
+      </c>
+      <c r="G167" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
         <v>233</v>
       </c>
-      <c r="D149">
-        <f t="array" ref="D149">MAX(LEN(D2:D147))</f>
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>340</v>
+      <c r="D169" t="e">
+        <f>MAX(LEN(D2:D167))</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -4916,10 +5658,257 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>292</v>
+      </c>
+      <c r="B14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B19" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>301</v>
+      </c>
+      <c r="B20" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>304</v>
+      </c>
+      <c r="B23" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>304</v>
+      </c>
+      <c r="B24" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>305</v>
+      </c>
+      <c r="B25" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>306</v>
+      </c>
+      <c r="B26" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>307</v>
+      </c>
+      <c r="B27" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>307</v>
+      </c>
+      <c r="B28" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4937,7 +5926,7 @@
         <v>237</v>
       </c>
       <c r="C1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5622,6 +6611,308 @@
       <c r="C58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_prerequisites` (edge_id, prerequisite_edge_id) VALUES (@MASTER_OF_ARMS_ID, @WEAPON_MASTER_ID);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>278</v>
+      </c>
+      <c r="B60" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>280</v>
+      </c>
+      <c r="B61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>282</v>
+      </c>
+      <c r="B62" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>283</v>
+      </c>
+      <c r="B63" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>289</v>
+      </c>
+      <c r="B65" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>293</v>
+      </c>
+      <c r="B66" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>295</v>
+      </c>
+      <c r="B67" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>298</v>
+      </c>
+      <c r="B68" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>304</v>
+      </c>
+      <c r="B69" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>310</v>
+      </c>
+      <c r="B70" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>312</v>
+      </c>
+      <c r="B71" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" t="s">
+        <v>316</v>
+      </c>
+      <c r="C72" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>238</v>
+      </c>
+      <c r="B74" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>316</v>
+      </c>
+      <c r="B77" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>325</v>
+      </c>
+      <c r="B78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>325</v>
+      </c>
+      <c r="B79" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" t="s">
+        <v>320</v>
+      </c>
+      <c r="C80" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>238</v>
+      </c>
+      <c r="B82" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>239</v>
+      </c>
+      <c r="B83" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>66</v>
+      </c>
+      <c r="B85" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>324</v>
+      </c>
+      <c r="B87" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>325</v>
+      </c>
+      <c r="B88" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>68</v>
+      </c>
+      <c r="B89" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>324</v>
+      </c>
+      <c r="B91" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>238</v>
+      </c>
+      <c r="B93" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>239</v>
+      </c>
+      <c r="B94" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>240</v>
+      </c>
+      <c r="B95" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>84</v>
+      </c>
+      <c r="B96" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -5630,12 +6921,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5651,13 +6942,13 @@
         <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5698,7 +6989,7 @@
         <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5713,7 +7004,7 @@
         <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5728,7 +7019,7 @@
         <v>244</v>
       </c>
       <c r="C6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5743,7 +7034,7 @@
         <v>247</v>
       </c>
       <c r="C7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5773,7 +7064,7 @@
         <v>242</v>
       </c>
       <c r="C9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5788,7 +7079,7 @@
         <v>245</v>
       </c>
       <c r="C10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5923,7 +7214,7 @@
         <v>245</v>
       </c>
       <c r="C19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6028,7 +7319,7 @@
         <v>245</v>
       </c>
       <c r="C26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6103,7 +7394,7 @@
         <v>246</v>
       </c>
       <c r="C31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6148,7 +7439,7 @@
         <v>244</v>
       </c>
       <c r="C34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6193,7 +7484,7 @@
         <v>244</v>
       </c>
       <c r="C37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6268,7 +7559,7 @@
         <v>245</v>
       </c>
       <c r="C42" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6283,7 +7574,7 @@
         <v>245</v>
       </c>
       <c r="C43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6313,7 +7604,7 @@
         <v>245</v>
       </c>
       <c r="C45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6358,7 +7649,7 @@
         <v>246</v>
       </c>
       <c r="C48" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6438,6 +7729,259 @@
       <c r="D53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO `edge_attribute_prerequisite` (edge, attribute_type, die_type) VALUES (@LIQUID_COURAGE_ID, 'VIGOR', 'D8');</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>278</v>
+      </c>
+      <c r="B55" t="s">
+        <v>246</v>
+      </c>
+      <c r="C55" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>280</v>
+      </c>
+      <c r="B56" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>288</v>
+      </c>
+      <c r="B57" t="s">
+        <v>242</v>
+      </c>
+      <c r="C57" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>288</v>
+      </c>
+      <c r="B58" t="s">
+        <v>244</v>
+      </c>
+      <c r="C58" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>293</v>
+      </c>
+      <c r="B59" t="s">
+        <v>246</v>
+      </c>
+      <c r="C59" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>304</v>
+      </c>
+      <c r="B60" t="s">
+        <v>242</v>
+      </c>
+      <c r="C60" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>306</v>
+      </c>
+      <c r="B61" t="s">
+        <v>246</v>
+      </c>
+      <c r="C61" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>309</v>
+      </c>
+      <c r="B62" t="s">
+        <v>246</v>
+      </c>
+      <c r="C62" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>309</v>
+      </c>
+      <c r="B63" t="s">
+        <v>247</v>
+      </c>
+      <c r="C63" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>315</v>
+      </c>
+      <c r="B64" t="s">
+        <v>242</v>
+      </c>
+      <c r="C64" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>315</v>
+      </c>
+      <c r="B65" t="s">
+        <v>245</v>
+      </c>
+      <c r="C65" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>317</v>
+      </c>
+      <c r="B66" t="s">
+        <v>247</v>
+      </c>
+      <c r="C66" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>320</v>
+      </c>
+      <c r="B67" t="s">
+        <v>246</v>
+      </c>
+      <c r="C67" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>324</v>
+      </c>
+      <c r="B68" t="s">
+        <v>245</v>
+      </c>
+      <c r="C68" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>324</v>
+      </c>
+      <c r="B69" t="s">
+        <v>246</v>
+      </c>
+      <c r="C69" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>325</v>
+      </c>
+      <c r="B70" t="s">
+        <v>245</v>
+      </c>
+      <c r="C70" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>326</v>
+      </c>
+      <c r="B71" t="s">
+        <v>245</v>
+      </c>
+      <c r="C71" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B72" t="s">
+        <v>242</v>
+      </c>
+      <c r="C72" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>327</v>
+      </c>
+      <c r="B73" t="s">
+        <v>245</v>
+      </c>
+      <c r="C73" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>327</v>
+      </c>
+      <c r="B74" t="s">
+        <v>247</v>
+      </c>
+      <c r="C74" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>328</v>
+      </c>
+      <c r="B75" t="s">
+        <v>242</v>
+      </c>
+      <c r="C75" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>328</v>
+      </c>
+      <c r="B76" t="s">
+        <v>245</v>
+      </c>
+      <c r="C76" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>330</v>
+      </c>
+      <c r="B77" t="s">
+        <v>245</v>
+      </c>
+      <c r="C77" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -6454,12 +7998,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6467,188 +8011,192 @@
     <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="133" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C8" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C11" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D13" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C15" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -6656,10 +8204,10 @@
         <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -6667,7 +8215,7 @@
         <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C18" t="s">
         <v>243</v>
@@ -6678,10 +8226,10 @@
         <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -6689,7 +8237,7 @@
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C20" t="s">
         <v>243</v>
@@ -6700,7 +8248,7 @@
         <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C21" t="s">
         <v>243</v>
@@ -6711,13 +8259,13 @@
         <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D22" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -6725,13 +8273,13 @@
         <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D23" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -6739,10 +8287,10 @@
         <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -6750,7 +8298,7 @@
         <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C25" t="s">
         <v>243</v>
@@ -6761,7 +8309,7 @@
         <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C26" t="s">
         <v>243</v>
@@ -6772,10 +8320,10 @@
         <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -6783,7 +8331,7 @@
         <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C28" t="s">
         <v>243</v>
@@ -6794,10 +8342,10 @@
         <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -6805,7 +8353,7 @@
         <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C30" t="s">
         <v>243</v>
@@ -6816,7 +8364,7 @@
         <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C31" t="s">
         <v>243</v>
@@ -6827,13 +8375,13 @@
         <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D32" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -6841,13 +8389,13 @@
         <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D33" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -6855,10 +8403,10 @@
         <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -6866,10 +8414,10 @@
         <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C35" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -6877,7 +8425,7 @@
         <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C36" t="s">
         <v>243</v>
@@ -6888,13 +8436,13 @@
         <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C37" t="s">
         <v>243</v>
       </c>
       <c r="D37" t="s">
-        <v>277</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -6902,10 +8450,10 @@
         <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -6913,7 +8461,7 @@
         <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C39" t="s">
         <v>243</v>
@@ -6924,7 +8472,7 @@
         <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C40" t="s">
         <v>243</v>
@@ -6935,10 +8483,10 @@
         <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6946,10 +8494,10 @@
         <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -6957,10 +8505,10 @@
         <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -6968,169 +8516,209 @@
         <v>105</v>
       </c>
       <c r="B44" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>282</v>
+      </c>
+      <c r="B46" t="s">
+        <v>257</v>
+      </c>
+      <c r="C46" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>283</v>
+      </c>
+      <c r="B47" t="s">
+        <v>257</v>
+      </c>
+      <c r="C47" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>288</v>
+      </c>
+      <c r="B49" t="s">
+        <v>251</v>
+      </c>
+      <c r="C49" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>303</v>
+      </c>
+      <c r="B50" t="s">
+        <v>257</v>
+      </c>
+      <c r="C50" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>310</v>
+      </c>
+      <c r="B51" t="s">
+        <v>252</v>
+      </c>
+      <c r="C51" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>312</v>
+      </c>
+      <c r="B52" t="s">
+        <v>252</v>
+      </c>
+      <c r="C52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" t="s">
+        <v>257</v>
+      </c>
+      <c r="C53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>315</v>
+      </c>
+      <c r="B54" t="s">
+        <v>252</v>
+      </c>
+      <c r="C54" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>324</v>
+      </c>
+      <c r="B55" t="s">
+        <v>269</v>
+      </c>
+      <c r="C55" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>325</v>
+      </c>
+      <c r="B56" t="s">
+        <v>269</v>
+      </c>
+      <c r="C56" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>326</v>
+      </c>
+      <c r="B57" t="s">
+        <v>345</v>
+      </c>
+      <c r="C57" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>326</v>
+      </c>
+      <c r="B58" t="s">
         <v>255</v>
       </c>
-      <c r="C44" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>252</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C58" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>253</v>
-      </c>
-      <c r="B51" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>254</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="D58" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>328</v>
+      </c>
+      <c r="B59" t="s">
+        <v>259</v>
+      </c>
+      <c r="C59" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>329</v>
+      </c>
+      <c r="B60" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>329</v>
+      </c>
+      <c r="B61" t="s">
+        <v>263</v>
+      </c>
+      <c r="C61" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>330</v>
+      </c>
+      <c r="B62" t="s">
+        <v>263</v>
+      </c>
+      <c r="C62" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>278</v>
-      </c>
-      <c r="B53" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>255</v>
-      </c>
-      <c r="B54" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>281</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B44">
-      <formula1>$A$50:$A$76</formula1>
+      <formula1>$A$53:$A$79</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C44">
-      <formula1>$B$50:$B$54</formula1>
+      <formula1>$B$53:$B$57</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>